<commit_message>
Title: Modified DSM for state, observer and strategy in the excel sheet Description: Packaged classes properly, created new json and added dv8 file
</commit_message>
<xml_diff>
--- a/src/main/java/edu/psu/behavioural/state/state.xlsx
+++ b/src/main/java/edu/psu/behavioural/state/state.xlsx
@@ -14,15 +14,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
-    <t>.\concreteState\TCPOctetStream.java</t>
-  </si>
-  <si>
-    <t>.\TCPState.java</t>
+    <t>.\states\TCPOctetStream.java</t>
   </si>
   <si>
     <t>.\context\TCPConnection.java</t>
   </si>
   <si>
+    <t>.\states\TCPState.java</t>
+  </si>
+  <si>
     <t>.\concreteState\TCPListen.java</t>
   </si>
   <si>
@@ -59,37 +59,37 @@
     <t>Import,Parameter</t>
   </si>
   <si>
+    <t>Import,Call:7,Contain,Parameter,Use:4</t>
+  </si>
+  <si>
+    <t>Import,Call,Use</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
     <t>Import,Call,Parameter:8</t>
   </si>
   <si>
-    <t>Import,Call:7,Contain,Parameter,Use:4</t>
-  </si>
-  <si>
-    <t>Import,Call,Use</t>
+    <t>Import,Call,Parameter</t>
   </si>
   <si>
     <t>Contain,Extend,Return,Import,Use:2</t>
   </si>
   <si>
-    <t>Import,Call,Parameter</t>
-  </si>
-  <si>
     <t>Call,Use</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
     <t>Import,Call:2,Parameter:2</t>
   </si>
   <si>
     <t>Create,Import,Call:4,Contain</t>
   </si>
   <si>
-    <t>Contain,Extend,Return,Import,Call,Use:2</t>
-  </si>
-  <si>
     <t>Import,Call,Parameter:2</t>
+  </si>
+  <si>
+    <t>Extend,Return,Import,Call,Contain,Use:2</t>
   </si>
 </sst>
 </file>
@@ -274,7 +274,9 @@
       <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -284,17 +286,15 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="I4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -305,16 +305,16 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s" s="10">
         <v>10</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="5"/>
@@ -327,16 +327,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G6" t="s" s="7">
         <v>11</v>
@@ -352,7 +352,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="E7" t="s">
+      <c r="D7" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="4"/>
@@ -377,10 +377,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" t="s" s="16">

</xml_diff>